<commit_message>
CRB Data Table and Picture
</commit_message>
<xml_diff>
--- a/Project/graphs/CRB.xlsx
+++ b/Project/graphs/CRB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rberi/Google Drive (Stanford GSB)/EdX &amp; Coursera/HarvardX/Advanced Topics in Data Science/2020-CS109B/Project/Graphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{74F29B91-F539-F74A-AB27-6EB6698C7F31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{8A9044CA-5790-A843-A655-47B598D4027D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940"/>
   </bookViews>
@@ -33,7 +33,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+  <si>
+    <t>Bias</t>
+  </si>
   <si>
     <t>Sersic Index</t>
   </si>
@@ -50,9 +53,6 @@
     <t>True Value</t>
   </si>
   <si>
-    <t>Prediction Bias</t>
-  </si>
-  <si>
     <t>Flux (in 100K)</t>
   </si>
   <si>
@@ -71,10 +71,10 @@
     <t>SNR=30 PSF=0.5 Sigma=400</t>
   </si>
   <si>
-    <t>Prediction SD</t>
-  </si>
-  <si>
     <t>Parameters</t>
+  </si>
+  <si>
+    <t>Std Dev</t>
   </si>
 </sst>
 </file>
@@ -83,7 +83,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -144,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +169,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -326,16 +332,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -345,13 +345,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -377,10 +370,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="4" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="4" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="5" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="5" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="3" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="5" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="5" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="4" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="4" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -696,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K31"/>
+  <dimension ref="B1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -707,359 +712,446 @@
     <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="9"/>
-      <c r="C2" s="27" t="s">
+    <row r="1" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:15" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="3"/>
+      <c r="C2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="2:15" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="7"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="22"/>
-    </row>
-    <row r="3" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="13"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="11" t="s">
+      <c r="H3" s="12" t="str">
+        <f>F3</f>
+        <v>Bias</v>
+      </c>
+      <c r="I3" s="13" t="str">
+        <f>G3</f>
+        <v>Std Dev</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="18">
         <v>1</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="19">
         <v>0.11</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="20">
         <f>1382.56311/100000</f>
         <v>1.3825631100000001E-2</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="21">
         <f>9048.004883/100000</f>
         <v>9.0480048829999993E-2</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="11"/>
-      <c r="C5" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="H4" s="20">
+        <v>0.11</v>
+      </c>
+      <c r="I4" s="21">
+        <v>-5.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B5" s="5"/>
+      <c r="C5" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="23">
         <v>3</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="24">
         <v>1.56</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="20">
         <v>1.041709</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="21">
         <v>0.74471699999999996</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="11"/>
-      <c r="C6" s="15" t="s">
+      <c r="H5" s="20">
+        <v>1.56</v>
+      </c>
+      <c r="I5" s="21">
+        <v>-0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B6" s="5"/>
+      <c r="C6" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="E6" s="24">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="F6" s="20">
+        <v>4.0960999999999997E-2</v>
+      </c>
+      <c r="G6" s="21">
+        <v>6.0809000000000002E-2</v>
+      </c>
+      <c r="H6" s="20">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="I6" s="21">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B7" s="5"/>
+      <c r="C7" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="23">
+        <v>-6.9000000000000006E-2</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0.11</v>
+      </c>
+      <c r="F7" s="20">
+        <v>-1.9592999999999999E-2</v>
+      </c>
+      <c r="G7" s="21">
+        <v>0.10245600000000001</v>
+      </c>
+      <c r="H7" s="20">
+        <v>0.11</v>
+      </c>
+      <c r="I7" s="21">
+        <v>-1.9E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B8" s="5"/>
+      <c r="C8" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="23">
+        <v>0.15</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0.11</v>
+      </c>
+      <c r="F8" s="20">
+        <v>-2.085E-2</v>
+      </c>
+      <c r="G8" s="21">
+        <v>9.8821999999999993E-2</v>
+      </c>
+      <c r="H8" s="20">
+        <v>0.11</v>
+      </c>
+      <c r="I8" s="21">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="26"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="23">
         <v>1</v>
       </c>
-      <c r="D6" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="E6" s="31">
+      <c r="E10" s="24">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="F6" s="2">
-        <v>4.0960999999999997E-2</v>
-      </c>
-      <c r="G6" s="8">
-        <v>6.0809000000000002E-2</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="11"/>
-      <c r="C7" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3">
-        <v>-6.9000000000000006E-2</v>
-      </c>
-      <c r="E7" s="31">
-        <v>0.11</v>
-      </c>
-      <c r="F7" s="2">
-        <v>-1.9592999999999999E-2</v>
-      </c>
-      <c r="G7" s="8">
-        <v>0.10245600000000001</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="11"/>
-      <c r="C8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="E8" s="31">
-        <v>0.11</v>
-      </c>
-      <c r="F8" s="2">
-        <v>-2.085E-2</v>
-      </c>
-      <c r="G8" s="8">
-        <v>9.8821999999999993E-2</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="10"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-      <c r="E10" s="31">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="F10" s="20">
         <f>-2191.242676/100000</f>
         <v>-2.1912426759999999E-2</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="21">
         <f>5793.616699/100000</f>
         <v>5.7936166990000003E-2</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="11"/>
-      <c r="C11" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="H10" s="20">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="I10" s="21">
+        <v>7.1999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B11" s="5"/>
+      <c r="C11" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="23">
         <v>3</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="24">
         <v>0.78</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="20">
         <v>0.83468200000000004</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="21">
         <v>0.78931700000000005</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="11"/>
-      <c r="C12" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3">
+      <c r="H11" s="20">
+        <v>-0.48</v>
+      </c>
+      <c r="I11" s="21">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B12" s="5"/>
+      <c r="C12" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="23">
         <v>0.3</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="24">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="20">
         <v>2.5010999999999999E-2</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="21">
         <v>3.5790000000000002E-2</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="11"/>
-      <c r="C13" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3">
+      <c r="H12" s="20">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="I12" s="21">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B13" s="5"/>
+      <c r="C13" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="23">
         <v>-6.9000000000000006E-2</v>
       </c>
-      <c r="E13" s="31">
+      <c r="E13" s="24">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="20">
         <v>1.1991999999999999E-2</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="21">
         <v>6.1041999999999999E-2</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="12"/>
-      <c r="C14" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="7">
+      <c r="H13" s="20">
+        <v>1E-3</v>
+      </c>
+      <c r="I13" s="21">
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="6"/>
+      <c r="C14" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="29">
         <v>0.15</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E14" s="30">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="31">
         <v>2.2680000000000001E-3</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="32">
         <v>5.6161999999999997E-2</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="20"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="19" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="27" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-    </row>
-    <row r="28" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-    </row>
-    <row r="29" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-    </row>
-    <row r="30" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-    </row>
-    <row r="31" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
+      <c r="H14" s="31">
+        <v>-2.7E-2</v>
+      </c>
+      <c r="I14" s="32">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="L16" s="1"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="L17" s="1"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="L18" s="1"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+    </row>
+    <row r="25" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+    </row>
+    <row r="26" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="L26" s="1"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+    </row>
+    <row r="27" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+    </row>
+    <row r="30" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+    </row>
+    <row r="31" spans="6:15" x14ac:dyDescent="0.2">
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>